<commit_message>
ai process log edited
</commit_message>
<xml_diff>
--- a/AI_Process_Log.xlsx
+++ b/AI_Process_Log.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N00233845\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N00233845\Documents\Emerging technologies\cinema-bookings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E214311-00CB-4818-BC6F-E28CC67EA00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38791BB0-599C-4AFD-B25D-D8077288EC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AI Process Log" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
   <si>
     <t>AI PROCESS LOG</t>
   </si>
@@ -166,6 +166,21 @@
   </si>
   <si>
     <t>got the ai to actually make the location page and try to fix the bookings also told it to "stylise the website"</t>
+  </si>
+  <si>
+    <t>Got the ai to fix the booking</t>
+  </si>
+  <si>
+    <t>Ai gave back the booking working completely fine now</t>
+  </si>
+  <si>
+    <t>Booking worked completely fine, all of the functionality is fine on the page</t>
+  </si>
+  <si>
+    <t>The ai is starting to make mistakes with its syntax, not sure if it’s the amount its trying to work it, the ai is forgetting to add { and ( to the end of its code causing errors I'd have to manually fix</t>
+  </si>
+  <si>
+    <t>Did the same tests as last time and went through the code myself to find what the ai was struggling with. Tried multiple times to get the ai to fix it itself however it just wasn’t able to</t>
   </si>
 </sst>
 </file>
@@ -286,20 +301,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,62 +635,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -685,118 +700,118 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="9"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
     </row>
     <row r="16" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -834,7 +849,7 @@
       <c r="A17" s="5">
         <v>1</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="6">
         <v>46056</v>
       </c>
       <c r="C17" s="3">
@@ -862,7 +877,7 @@
       <c r="A18" s="5">
         <v>2</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="6">
         <v>46057</v>
       </c>
       <c r="C18" s="3">
@@ -892,7 +907,7 @@
       <c r="A19" s="5">
         <v>3</v>
       </c>
-      <c r="B19" s="12">
+      <c r="B19" s="6">
         <v>46057</v>
       </c>
       <c r="C19" s="3">
@@ -922,14 +937,30 @@
       <c r="A20" s="5">
         <v>4</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="B20" s="6">
+        <v>46057</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="J20" s="3"/>
     </row>
     <row r="21" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
@@ -1578,12 +1609,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="A13:K13"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="B5:D5"/>
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="A4:K4"/>
@@ -1592,21 +1617,18 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="A12:K12"/>
     <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DF200B604F543D4E96F8CC7C901240C3" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="65cac28d9b88990158ba4af9b48a7352">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a14edb67-64d8-4b5b-8995-e266d62a7d22" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="796dc2f3a0be1b865fd6b38ecd54e07c" ns2:_="">
     <xsd:import namespace="a14edb67-64d8-4b5b-8995-e266d62a7d22"/>
@@ -1744,6 +1766,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1751,14 +1782,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{786E9469-6AE4-4683-B620-D6446712212D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4203073-7FF2-4136-A5EA-B189D8F74362}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1776,6 +1799,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{786E9469-6AE4-4683-B620-D6446712212D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62EF381A-753F-4574-BF74-42D6AF83CA80}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
fifth and sixth iterations
</commit_message>
<xml_diff>
--- a/AI_Process_Log.xlsx
+++ b/AI_Process_Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29808"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\N00233845\Documents\Emerging technologies\cinema-bookings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EAFB68-4B3E-4ADB-BEF8-1804BA606DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B15052F-4F82-44E4-9D55-077353463A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3660" yWindow="795" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,17 +27,16 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="93">
   <si>
     <t>AI PROCESS LOG</t>
   </si>
@@ -252,23 +251,77 @@
     <t>Asked copilot to add a register and login page</t>
   </si>
   <si>
+    <t>Created the login and register page functionality with buttons to register or login</t>
+  </si>
+  <si>
+    <t>functionality of the webpage worked perfectly fine</t>
+  </si>
+  <si>
     <t>the buttons for the page were completely different from the rest of the formatting of the page</t>
   </si>
   <si>
-    <t>Created the login and register page functionality with buttons to register or login</t>
-  </si>
-  <si>
-    <t>functionality of the webpage worked perfectly fine</t>
-  </si>
-  <si>
     <t>tested both the login and register to make sure they were working fine</t>
+  </si>
+  <si>
+    <t>OpenCodeAI</t>
+  </si>
+  <si>
+    <t>Asked OpenCode to just add whatever functions it wants to add that it thinks a user that has logged in should do</t>
+  </si>
+  <si>
+    <t>The AI added loads of features, User profile, Filter System, Reviews, rating system, favourites, pre ordering concessions, promotional codes, booking history and even made it so that the user data gets saved in localStorage</t>
+  </si>
+  <si>
+    <t>The user dashboard worked, comments worked partially, concessions ordering worked fine and viewing bookings that had been made was fine</t>
+  </si>
+  <si>
+    <t>Users were still able to make multiple bookings for the same seats, comments couldnt be deleted. only updated</t>
+  </si>
+  <si>
+    <t>I went through all the features, seeing if i could comment twice, and checked if the bookings changed anything in the seating once had booked</t>
+  </si>
+  <si>
+    <t>might be a few features i forgot to check or glossed over as im not completely sure what the ai added</t>
+  </si>
+  <si>
+    <t>Got openCode to remake the website's design, and add more cinema data</t>
+  </si>
+  <si>
+    <t>The ai added filtering to the map, redesigned the page entirely.</t>
+  </si>
+  <si>
+    <t>browsing the website worked but thats about it</t>
+  </si>
+  <si>
+    <t>The search function didnt work at all nor the filtering, a notifcation would just come up saying what it was filtering for, it also deleted the images i had put in for copilot to use whenever i clicked on details on the map it would also put my user name in the search bar. when the ai was trying to create info for one of the movies there were multiple directors and the ai didnt but them in an array</t>
+  </si>
+  <si>
+    <t>went through the entire page and carefully checked every detail that the ai had said it had changed</t>
+  </si>
+  <si>
+    <t>Got the ai to fix whatever errors it had and to remove any buttons that were useless</t>
+  </si>
+  <si>
+    <t>the ai removed most of the buttons and completely fixed the search function and made it so that you can search by director</t>
+  </si>
+  <si>
+    <t>practically everything worked perfectly fine to the point that even made it so that the user can search by director and rating</t>
+  </si>
+  <si>
+    <t>The map is still a bit broken when clicking on details for the cinema it will just zoom in on the point on the map</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Messed with the search engine to see what details the user can search with and i rechecked the map </t>
+  </si>
+  <si>
+    <t>Might've missed a button or two that the ai had put in that i hadnt noticed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,17 +438,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,11 +754,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="3" width="12" customWidth="1"/>
@@ -715,8 +768,8 @@
     <col min="8" max="11" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:11" ht="30" customHeight="1">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
@@ -730,8 +783,8 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:11" ht="15.75">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="8"/>
@@ -745,8 +798,8 @@
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:11">
+      <c r="A4" s="11" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="8"/>
@@ -760,7 +813,7 @@
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -777,7 +830,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -798,7 +851,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -819,8 +872,8 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:11">
+      <c r="A9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="8"/>
@@ -834,8 +887,8 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+    <row r="10" spans="1:11" ht="39.950000000000003" customHeight="1">
+      <c r="A10" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="9"/>
@@ -849,8 +902,8 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:11">
+      <c r="A12" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="8"/>
@@ -864,8 +917,8 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:11" ht="30" customHeight="1">
+      <c r="A13" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="9"/>
@@ -879,8 +932,8 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:11">
+      <c r="A15" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="8"/>
@@ -894,7 +947,7 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="35.1" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>18</v>
       </c>
@@ -926,7 +979,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="60" customHeight="1">
       <c r="A17" s="4">
         <v>1</v>
       </c>
@@ -954,7 +1007,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
-    <row r="18" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="60" customHeight="1">
       <c r="A18" s="4">
         <v>2</v>
       </c>
@@ -984,7 +1037,7 @@
       </c>
       <c r="J18" s="6"/>
     </row>
-    <row r="19" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="60" customHeight="1">
       <c r="A19" s="4">
         <v>3</v>
       </c>
@@ -1014,7 +1067,7 @@
       </c>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="60" customHeight="1">
       <c r="A20" s="4">
         <v>4</v>
       </c>
@@ -1044,7 +1097,7 @@
       </c>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="60" customHeight="1">
       <c r="A21" s="4">
         <v>5</v>
       </c>
@@ -1074,7 +1127,7 @@
       </c>
       <c r="J21" s="6"/>
     </row>
-    <row r="22" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="60" customHeight="1">
       <c r="A22" s="4">
         <v>6</v>
       </c>
@@ -1104,7 +1157,7 @@
       </c>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="60" customHeight="1">
       <c r="A23" s="4">
         <v>7</v>
       </c>
@@ -1136,7 +1189,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="60" customHeight="1">
       <c r="A24" s="4">
         <v>8</v>
       </c>
@@ -1168,7 +1221,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="60" customHeight="1">
       <c r="A25" s="4">
         <v>9</v>
       </c>
@@ -1185,62 +1238,114 @@
         <v>70</v>
       </c>
       <c r="F25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="H25" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="I25" s="6" t="s">
         <v>74</v>
       </c>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="60" customHeight="1">
       <c r="A26" s="4">
         <v>10</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="5">
+        <v>46062</v>
+      </c>
+      <c r="C26" s="6">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="60" customHeight="1">
       <c r="A27" s="4">
         <v>11</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="B27" s="5">
+        <v>46062</v>
+      </c>
+      <c r="C27" s="6">
+        <v>6</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>86</v>
+      </c>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="60" customHeight="1">
       <c r="A28" s="4">
         <v>12</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5">
+        <v>46062</v>
+      </c>
+      <c r="C28" s="6">
+        <v>6</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="60" customHeight="1">
       <c r="A29" s="4">
         <v>13</v>
       </c>
@@ -1254,7 +1359,7 @@
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
-    <row r="30" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="60" customHeight="1">
       <c r="A30" s="4">
         <v>14</v>
       </c>
@@ -1268,7 +1373,7 @@
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
     </row>
-    <row r="31" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="60" customHeight="1">
       <c r="A31" s="4">
         <v>15</v>
       </c>
@@ -1282,7 +1387,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
     </row>
-    <row r="32" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="60" customHeight="1">
       <c r="A32" s="4">
         <v>16</v>
       </c>
@@ -1296,7 +1401,7 @@
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
     </row>
-    <row r="33" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="60" customHeight="1">
       <c r="A33" s="4">
         <v>17</v>
       </c>
@@ -1310,7 +1415,7 @@
       <c r="I33" s="6"/>
       <c r="J33" s="6"/>
     </row>
-    <row r="34" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="60" customHeight="1">
       <c r="A34" s="4">
         <v>18</v>
       </c>
@@ -1324,7 +1429,7 @@
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
     </row>
-    <row r="35" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="60" customHeight="1">
       <c r="A35" s="4">
         <v>19</v>
       </c>
@@ -1338,7 +1443,7 @@
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
     </row>
-    <row r="36" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="60" customHeight="1">
       <c r="A36" s="4">
         <v>20</v>
       </c>
@@ -1352,7 +1457,7 @@
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
     </row>
-    <row r="37" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" ht="60" customHeight="1">
       <c r="A37" s="4">
         <v>21</v>
       </c>
@@ -1366,7 +1471,7 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
     </row>
-    <row r="38" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="60" customHeight="1">
       <c r="A38" s="4">
         <v>22</v>
       </c>
@@ -1380,7 +1485,7 @@
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
     </row>
-    <row r="39" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="60" customHeight="1">
       <c r="A39" s="4">
         <v>23</v>
       </c>
@@ -1394,7 +1499,7 @@
       <c r="I39" s="6"/>
       <c r="J39" s="6"/>
     </row>
-    <row r="40" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" ht="60" customHeight="1">
       <c r="A40" s="4">
         <v>24</v>
       </c>
@@ -1408,7 +1513,7 @@
       <c r="I40" s="6"/>
       <c r="J40" s="6"/>
     </row>
-    <row r="41" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="60" customHeight="1">
       <c r="A41" s="4">
         <v>25</v>
       </c>
@@ -1422,7 +1527,7 @@
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
     </row>
-    <row r="42" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="60" customHeight="1">
       <c r="A42" s="4">
         <v>26</v>
       </c>
@@ -1436,7 +1541,7 @@
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
     </row>
-    <row r="43" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="60" customHeight="1">
       <c r="A43" s="4">
         <v>27</v>
       </c>
@@ -1450,7 +1555,7 @@
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
     </row>
-    <row r="44" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="60" customHeight="1">
       <c r="A44" s="4">
         <v>28</v>
       </c>
@@ -1464,7 +1569,7 @@
       <c r="I44" s="6"/>
       <c r="J44" s="6"/>
     </row>
-    <row r="45" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="60" customHeight="1">
       <c r="A45" s="4">
         <v>29</v>
       </c>
@@ -1478,7 +1583,7 @@
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
     </row>
-    <row r="46" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="60" customHeight="1">
       <c r="A46" s="4">
         <v>30</v>
       </c>
@@ -1492,7 +1597,7 @@
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
     </row>
-    <row r="47" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="60" customHeight="1">
       <c r="A47" s="4">
         <v>31</v>
       </c>
@@ -1506,7 +1611,7 @@
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
     </row>
-    <row r="48" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="60" customHeight="1">
       <c r="A48" s="4">
         <v>32</v>
       </c>
@@ -1520,7 +1625,7 @@
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
     </row>
-    <row r="49" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" ht="60" customHeight="1">
       <c r="A49" s="4">
         <v>33</v>
       </c>
@@ -1534,7 +1639,7 @@
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
     </row>
-    <row r="50" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="60" customHeight="1">
       <c r="A50" s="4">
         <v>34</v>
       </c>
@@ -1548,7 +1653,7 @@
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
     </row>
-    <row r="51" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="60" customHeight="1">
       <c r="A51" s="4">
         <v>35</v>
       </c>
@@ -1562,7 +1667,7 @@
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
     </row>
-    <row r="52" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" ht="60" customHeight="1">
       <c r="A52" s="4">
         <v>36</v>
       </c>
@@ -1576,7 +1681,7 @@
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
     </row>
-    <row r="53" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="60" customHeight="1">
       <c r="A53" s="4">
         <v>37</v>
       </c>
@@ -1590,7 +1695,7 @@
       <c r="I53" s="6"/>
       <c r="J53" s="6"/>
     </row>
-    <row r="54" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="60" customHeight="1">
       <c r="A54" s="4">
         <v>38</v>
       </c>
@@ -1604,7 +1709,7 @@
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
     </row>
-    <row r="55" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="60" customHeight="1">
       <c r="A55" s="4">
         <v>39</v>
       </c>
@@ -1618,7 +1723,7 @@
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
     </row>
-    <row r="56" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="60" customHeight="1">
       <c r="A56" s="4">
         <v>40</v>
       </c>
@@ -1632,7 +1737,7 @@
       <c r="I56" s="6"/>
       <c r="J56" s="6"/>
     </row>
-    <row r="57" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" ht="60" customHeight="1">
       <c r="A57" s="4">
         <v>41</v>
       </c>
@@ -1646,7 +1751,7 @@
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
     </row>
-    <row r="58" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="60" customHeight="1">
       <c r="A58" s="4">
         <v>42</v>
       </c>
@@ -1660,7 +1765,7 @@
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
     </row>
-    <row r="59" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="60" customHeight="1">
       <c r="A59" s="4">
         <v>43</v>
       </c>
@@ -1674,7 +1779,7 @@
       <c r="I59" s="6"/>
       <c r="J59" s="6"/>
     </row>
-    <row r="60" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="60" customHeight="1">
       <c r="A60" s="4">
         <v>44</v>
       </c>
@@ -1688,7 +1793,7 @@
       <c r="I60" s="6"/>
       <c r="J60" s="6"/>
     </row>
-    <row r="61" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" ht="60" customHeight="1">
       <c r="A61" s="4">
         <v>45</v>
       </c>
@@ -1702,7 +1807,7 @@
       <c r="I61" s="6"/>
       <c r="J61" s="6"/>
     </row>
-    <row r="62" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="60" customHeight="1">
       <c r="A62" s="4">
         <v>46</v>
       </c>
@@ -1716,7 +1821,7 @@
       <c r="I62" s="6"/>
       <c r="J62" s="6"/>
     </row>
-    <row r="63" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="60" customHeight="1">
       <c r="A63" s="4">
         <v>47</v>
       </c>
@@ -1730,7 +1835,7 @@
       <c r="I63" s="6"/>
       <c r="J63" s="6"/>
     </row>
-    <row r="64" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="60" customHeight="1">
       <c r="A64" s="4">
         <v>48</v>
       </c>
@@ -1744,7 +1849,7 @@
       <c r="I64" s="6"/>
       <c r="J64" s="6"/>
     </row>
-    <row r="65" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="60" customHeight="1">
       <c r="A65" s="4">
         <v>49</v>
       </c>
@@ -1758,7 +1863,7 @@
       <c r="I65" s="6"/>
       <c r="J65" s="6"/>
     </row>
-    <row r="66" spans="1:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="60" customHeight="1">
       <c r="A66" s="4">
         <v>50</v>
       </c>
@@ -1774,12 +1879,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="A13:K13"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="A10:K10"/>
-    <mergeCell ref="B5:D5"/>
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="A4:K4"/>
@@ -1788,18 +1887,21 @@
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="A12:K12"/>
     <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="A13:K13"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1941,42 +2043,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{786E9469-6AE4-4683-B620-D6446712212D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62EF381A-753F-4574-BF74-42D6AF83CA80}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4203073-7FF2-4136-A5EA-B189D8F74362}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a14edb67-64d8-4b5b-8995-e266d62a7d22"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4203073-7FF2-4136-A5EA-B189D8F74362}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62EF381A-753F-4574-BF74-42D6AF83CA80}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{786E9469-6AE4-4683-B620-D6446712212D}"/>
 </file>
</xml_diff>